<commit_message>
CampusTestData.xlsx -> DiscountSheet added Discounts.feature added DiscountSteps.java added DialogPage.java any Locators added LeftBar.java ayn Locators added
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/CampusTestData.xlsx
+++ b/src/test/java/ApachePOI/CampusTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\merys.io-Ben\src\test\java\ApachePOI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4193B184-4D71-4C91-8F7A-CE61B47F7E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96EC893-4D08-454C-8C5E-1282855D4EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BankAccounts" sheetId="1" r:id="rId1"/>
     <sheet name="Nationalities" sheetId="2" r:id="rId2"/>
+    <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Hans Müller</t>
   </si>
@@ -110,6 +111,66 @@
   </si>
   <si>
     <t>English775</t>
+  </si>
+  <si>
+    <t>EnglishCourse</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>GermanCourse</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>FranceCourse</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>TechnicalCourse</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>MathCourse</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>CulturCourse</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>TestNGCourse</t>
+  </si>
+  <si>
+    <t>CucumberCourse</t>
+  </si>
+  <si>
+    <t>JavaCourse</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>PostmanCourse</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>MySQLCourse</t>
+  </si>
+  <si>
+    <t>JenkinsCourse</t>
   </si>
 </sst>
 </file>
@@ -549,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF46FAE4-FC55-4608-A678-C19C4B411CF4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -594,4 +655,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68F74F1-285C-47F1-844C-2A72C4046838}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SchoolDepartment.xlsx deleted SchoolDepartments.java -> Bug Fixed SchoolDepartment.feature -> BUG Fixed
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/CampusTestData.xlsx
+++ b/src/test/java/ApachePOI/CampusTestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\merys.io-Ben\src\test\java\ApachePOI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\mersys.io\src\test\java\ApachePOI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96EC893-4D08-454C-8C5E-1282855D4EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B72C9C-30EC-46AC-BD02-B22128E9E7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BankAccounts" sheetId="1" r:id="rId1"/>
     <sheet name="Nationalities" sheetId="2" r:id="rId2"/>
     <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
+    <sheet name="SchoolDepartment" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Hans Müller</t>
   </si>
@@ -171,6 +172,18 @@
   </si>
   <si>
     <t>JenkinsCourse</t>
+  </si>
+  <si>
+    <t>ben</t>
+  </si>
+  <si>
+    <t>sen</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Sdet</t>
   </si>
 </sst>
 </file>
@@ -661,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68F74F1-285C-47F1-844C-2A72C4046838}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -795,4 +808,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3877CC42-9B82-435D-99F7-A82CA68B36BE}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DocumentTypes.feature -> added DocumentTypesSteps.java -> added DialogPage.java any Locators -> added LeftBar.java any Locators -> added
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/CampusTestData.xlsx
+++ b/src/test/java/ApachePOI/CampusTestData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\mersys.io\src\test\java\ApachePOI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B72C9C-30EC-46AC-BD02-B22128E9E7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB00152-91FE-410B-A360-D922FE7D80E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BankAccounts" sheetId="1" r:id="rId1"/>
     <sheet name="Nationalities" sheetId="2" r:id="rId2"/>
     <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
     <sheet name="SchoolDepartment" sheetId="4" r:id="rId4"/>
+    <sheet name="DocumentTypes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Hans Müller</t>
   </si>
@@ -184,6 +185,33 @@
   </si>
   <si>
     <t>Sdet</t>
+  </si>
+  <si>
+    <t>ID card</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>Driver's license</t>
+  </si>
+  <si>
+    <t>is required</t>
+  </si>
+  <si>
+    <t>is not required</t>
+  </si>
+  <si>
+    <t>employment contract</t>
+  </si>
+  <si>
+    <t>rental contract</t>
+  </si>
+  <si>
+    <t>vehicle registration</t>
+  </si>
+  <si>
+    <t>is  required</t>
   </si>
 </sst>
 </file>
@@ -814,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3877CC42-9B82-435D-99F7-A82CA68B36BE}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -839,4 +867,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54C302E-0662-4BB9-BC45-4951ED9E4FF4}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>